<commit_message>
minor cleanup files in dev folder
</commit_message>
<xml_diff>
--- a/dev/SPEED/speedtable_1k_500.xlsx
+++ b/dev/SPEED/speedtable_1k_500.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorrale\R\mysource\EJAM\inst\SPEED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorrale\R\mysource\EJAM\dev\SPEED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497DA746-1D2D-4CC4-B11F-D476C05D127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8855F4F-AAC2-4F67-A43E-B02EBA59F3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="data" sheetId="1" r:id="rId4"/>
     <sheet name="Chart4" sheetId="6" r:id="rId5"/>
     <sheet name="blockcount" sheetId="4" r:id="rId6"/>
+    <sheet name="PLOTS" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6365,7 +6366,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{01ABFC24-A85F-4EEA-AE54-7C5D0E523287}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6376,7 +6377,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{771EA786-CAAA-4877-9E1E-AB65E138D30B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6387,7 +6388,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{531B9EA9-D6EB-49E0-A911-3B780BD968E5}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6400,7 +6401,7 @@
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="127" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6411,7 +6412,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665221" cy="6288186"/>
+    <xdr:ext cx="8670000" cy="6300000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6764,7 +6765,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665221" cy="6288186"/>
+    <xdr:ext cx="8670000" cy="6300000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7053,7 +7054,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8665221" cy="6288186"/>
+    <xdr:ext cx="8670000" cy="6300000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7127,7 +7128,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669364" cy="6296186"/>
+    <xdr:ext cx="8670000" cy="6300000"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7976,6 +7977,194 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6384DC7-9686-8C64-E459-6D4F158CF035}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="381000"/>
+          <a:ext cx="9058275" cy="6334125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B232CA82-D7F0-5B52-BAF3-E711E39E0A15}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10363200" y="381000"/>
+          <a:ext cx="9020175" cy="6353175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BDA60EE-3711-D888-27F6-310B8DFEE31F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="7048500"/>
+          <a:ext cx="10239375" cy="6219825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}" name="Table2" displayName="Table2" ref="B3:C8" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="B3:C8" xr:uid="{E04C2DA1-EF8F-4E90-B733-8EC6D32CF1BE}"/>
@@ -8290,7 +8479,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:M6"/>
+      <selection activeCell="A9" sqref="A9:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9278,7 +9467,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9730,4 +9919,19 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD397FD3-DE43-4575-9CEB-2086EDB47665}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S38" sqref="S38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>